<commit_message>
update SDs for R4, remove all logical defs
</commit_message>
<xml_diff>
--- a/docs/extension-modality.xlsx
+++ b/docs/extension-modality.xlsx
@@ -147,7 +147,7 @@
 </t>
   </si>
   <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
   </si>
   <si>
@@ -158,10 +158,10 @@
 </t>
   </si>
   <si>
-    <t>xml:id (or equivalent in JSON)</t>
-  </si>
-  <si>
-    <t>unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+    <t>Unique id for inter-element referencing</t>
+  </si>
+  <si>
+    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
   </si>
   <si>
     <t>Element.id</t>
@@ -181,10 +181,10 @@
 </t>
   </si>
   <si>
-    <t>Additional Content defined by implementations</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. In order to make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+    <t>Additional content defined by implementations</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
   </si>
   <si>
     <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
@@ -219,13 +219,13 @@
     <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
   </si>
   <si>
-    <t>http://www.fhir.org/guides/mfhir/StructureDefinition/extension-modality</t>
+    <t>http://www.fhir.org/guides/omhtofhir/StructureDefinition/extension-modality</t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>Extension.valueCode</t>
+    <t>Extension.value[x]</t>
   </si>
   <si>
     <t xml:space="preserve">code
@@ -235,16 +235,17 @@
     <t>Value of extension</t>
   </si>
   <si>
-    <t>Value of extension - may be a resource or one of a constrained set of the data types (see Extensibility in the spec for list).</t>
+    <t>Value of extension - must be one of a constrained set of the data types (see [Extensibility](http://hl7.org/fhir/R4/extensibility.html) for a list).</t>
   </si>
   <si>
     <t>required</t>
   </si>
   <si>
-    <t>http://www.fhir.org/guides/mfhir/ValueSet/modality-codes</t>
-  </si>
-  <si>
-    <t>Extension.value[x]</t>
+    <t>http://www.fhir.org/guides/omhtofhir/ValueSet/modality-codes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+</t>
   </si>
 </sst>
 </file>
@@ -402,7 +403,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="19.53515625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="19.03125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.34765625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="12.19921875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
@@ -426,7 +427,7 @@
     <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="73.37890625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="54.82421875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="58.90234375" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="40.0859375" customWidth="true" bestFit="true"/>
@@ -846,7 +847,7 @@
         <v>37</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="AJ4" t="s" s="2">
         <v>49</v>
@@ -1036,7 +1037,7 @@
         <v>37</v>
       </c>
       <c r="AE6" t="s" s="2">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="AF6" t="s" s="2">
         <v>38</v>
@@ -1048,7 +1049,7 @@
         <v>37</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="AJ6" t="s" s="2">
         <v>66</v>

</xml_diff>